<commit_message>
Only 1 query left
</commit_message>
<xml_diff>
--- a/A2/DBMS Lab SQL Assignment 2.xlsx
+++ b/A2/DBMS Lab SQL Assignment 2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="181">
   <si>
     <t>Entities</t>
   </si>
@@ -438,6 +438,12 @@
     <t>24/12/2022 18:30:00</t>
   </si>
   <si>
+    <t>19/12/2022 10:30:00</t>
+  </si>
+  <si>
+    <t>23/12/2022 10:30:00</t>
+  </si>
+  <si>
     <t>PrimaryAffiliation</t>
   </si>
   <si>
@@ -523,6 +529,9 @@
   </si>
   <si>
     <t>07/05/2028 18:30:00</t>
+  </si>
+  <si>
+    <t>19/12/2022 13:00:00</t>
   </si>
   <si>
     <t>09/07/2013 10:30:00</t>
@@ -2408,11 +2417,21 @@
       <c r="G49" s="17"/>
       <c r="H49" s="29"/>
       <c r="I49" s="29"/>
-      <c r="K49" s="17"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="28"/>
-      <c r="N49" s="28"/>
-      <c r="O49" s="28"/>
+      <c r="K49" s="18">
+        <v>123.0</v>
+      </c>
+      <c r="L49" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="M49" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="N49" s="19">
+        <v>200.0</v>
+      </c>
+      <c r="O49" s="19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="B50" s="18">
@@ -2628,11 +2647,21 @@
       </c>
     </row>
     <row r="68">
-      <c r="B68" s="17"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
+      <c r="B68" s="18">
+        <v>7.0</v>
+      </c>
+      <c r="C68" s="18">
+        <v>2.0231425E7</v>
+      </c>
+      <c r="D68" s="19">
+        <v>123.0</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="69">
       <c r="B69" s="17"/>
@@ -2731,6 +2760,7 @@
     <col customWidth="1" min="5" max="5" width="23.13"/>
     <col customWidth="1" min="10" max="10" width="17.25"/>
     <col customWidth="1" min="12" max="12" width="16.25"/>
+    <col customWidth="1" min="15" max="15" width="20.5"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -2787,7 +2817,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>10</v>
@@ -2814,13 +2844,13 @@
         <v>8</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="P6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7">
@@ -2859,10 +2889,10 @@
         <v>400.0</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L8" s="19">
         <v>40017.0</v>
@@ -2880,7 +2910,7 @@
         <v>1.0</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9">
@@ -2903,10 +2933,10 @@
         <v>100.0</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L9" s="22">
         <v>10013.0</v>
@@ -2924,7 +2954,7 @@
         <v>2.0</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10">
@@ -2947,10 +2977,10 @@
         <v>500.0</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L10" s="31">
         <v>50033.0</v>
@@ -2968,7 +2998,7 @@
         <v>3.0</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11">
@@ -2991,10 +3021,10 @@
         <v>300.0</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L11" s="22">
         <v>30023.0</v>
@@ -3012,7 +3042,7 @@
         <v>4.0</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12">
@@ -3035,10 +3065,10 @@
         <v>400.0</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L12" s="22">
         <v>40019.0</v>
@@ -3056,7 +3086,7 @@
         <v>5.0</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13">
@@ -3079,10 +3109,10 @@
         <v>100.0</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L13" s="22">
         <v>10022.0</v>
@@ -3100,7 +3130,7 @@
         <v>6.0</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14">
@@ -3123,10 +3153,10 @@
         <v>300.0</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L14" s="31">
         <v>30023.0</v>
@@ -3144,7 +3174,7 @@
         <v>7.0</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15">
@@ -3188,7 +3218,7 @@
         <v>8.0</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16">
@@ -3222,7 +3252,7 @@
         <v>9.0</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17">
@@ -3256,7 +3286,7 @@
         <v>10.0</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18">
@@ -3319,13 +3349,13 @@
         <v>16</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>13</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24">
@@ -3333,13 +3363,13 @@
         <v>13</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
@@ -3363,7 +3393,7 @@
         <v>1.0</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="K25" s="27">
         <v>30023.0</v>
@@ -3380,10 +3410,10 @@
         <v>213.0</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G26" s="17">
         <v>2.0231436E7</v>
@@ -3395,7 +3425,7 @@
         <v>2.0</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K26" s="27">
         <v>30023.0</v>
@@ -3412,10 +3442,10 @@
         <v>213.0</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G27" s="22">
         <v>2.0231372E7</v>
@@ -3427,7 +3457,7 @@
         <v>3.0</v>
       </c>
       <c r="J27" s="33" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K27" s="24">
         <v>10013.0</v>
@@ -3444,10 +3474,10 @@
         <v>213.0</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G28" s="18">
         <v>2.0231356E7</v>
@@ -3459,7 +3489,7 @@
         <v>4.0</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K28" s="19">
         <v>40017.0</v>
@@ -3476,10 +3506,10 @@
         <v>177.0</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G29" s="17">
         <v>2.0231396E7</v>
@@ -3491,7 +3521,7 @@
         <v>5.0</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="K29" s="26">
         <v>50033.0</v>
@@ -3508,10 +3538,10 @@
         <v>177.0</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G30" s="17">
         <v>2.0231412E7</v>
@@ -3523,7 +3553,7 @@
         <v>6.0</v>
       </c>
       <c r="J30" s="20" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K30" s="19">
         <v>10022.0</v>
@@ -3540,17 +3570,29 @@
         <v>132.0</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
+        <v>171</v>
+      </c>
+      <c r="G31" s="18">
+        <v>2.0231425E7</v>
+      </c>
+      <c r="H31" s="19">
+        <v>132.0</v>
+      </c>
+      <c r="I31" s="19">
+        <v>7.0</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="K31" s="19">
+        <v>50033.0</v>
+      </c>
+      <c r="L31" s="19">
+        <v>170039.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="18">
@@ -3560,10 +3602,10 @@
         <v>165.0</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="29"/>
@@ -3580,10 +3622,10 @@
         <v>303.0</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="29"/>
@@ -3600,10 +3642,10 @@
         <v>303.0</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="29"/>
@@ -3620,10 +3662,10 @@
         <v>177.0</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>